<commit_message>
Analysis of #-pred-v and #-pred-v-adv-v etc.
</commit_message>
<xml_diff>
--- a/R_files/Rresults/zscoresStepwise_Oct1.xlsx
+++ b/R_files/Rresults/zscoresStepwise_Oct1.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="190" windowWidth="19140" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="190" windowWidth="19140" windowHeight="7770" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="main record" sheetId="1" r:id="rId1"/>
     <sheet name="working" sheetId="2" r:id="rId2"/>
-    <sheet name="#-pred-v" sheetId="3" r:id="rId3"/>
+    <sheet name="#-pred-v-auxy" sheetId="3" r:id="rId3"/>
+    <sheet name="#-pred-v-adv-v" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="566">
   <si>
     <t>Aeschylus</t>
   </si>
@@ -1693,6 +1694,27 @@
   </si>
   <si>
     <t>#-pred-v-auxy-d/pred-v</t>
+  </si>
+  <si>
+    <t>#-pred-v-auxy-c / pred-v</t>
+  </si>
+  <si>
+    <t>#-pred-v-auxy-d-auxz-d / pred-v-auxy-d</t>
+  </si>
+  <si>
+    <t>sum of # 3 and #111 as % of # 2</t>
+  </si>
+  <si>
+    <t>sum of # 3 and # 11 as % of total</t>
+  </si>
+  <si>
+    <t>#-pred-v-adv-v / #-pred-v</t>
+  </si>
+  <si>
+    <t>#-pred-v-adv-v-obj-n / #-pred-v-adv-v</t>
+  </si>
+  <si>
+    <t>#-pred-v-adv-v-obj-n-atr-a / #-pred-v-adv-v-obj-n</t>
   </si>
 </sst>
 </file>
@@ -2177,8 +2199,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2523,11 +2548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AOI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="HK3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="HM16" sqref="HM16"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51507,10 +51532,10 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -52529,21 +52554,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -52711,20 +52736,1298 @@
         <v>-1.26922079789228</v>
       </c>
     </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>558</v>
+      </c>
+      <c r="L20" t="s">
+        <v>559</v>
+      </c>
+      <c r="P20" t="s">
+        <v>562</v>
+      </c>
+      <c r="U20" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>550</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>553</v>
+      </c>
+      <c r="F22" t="s">
+        <v>554</v>
+      </c>
+      <c r="H22">
+        <v>111</v>
+      </c>
+      <c r="I22">
+        <v>111</v>
+      </c>
+      <c r="L22" t="s">
+        <v>553</v>
+      </c>
+      <c r="M22" t="s">
+        <v>554</v>
+      </c>
+      <c r="P22" t="s">
+        <v>553</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>554</v>
+      </c>
+      <c r="U22" t="s">
+        <v>553</v>
+      </c>
+      <c r="V22" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>551</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>3.6585365853658498</v>
+      </c>
+      <c r="C24">
+        <v>0.120103385276993</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E36" si="0">B24/B3</f>
+        <v>0.62090947726306756</v>
+      </c>
+      <c r="F24">
+        <f>STANDARDIZE(E24,$E$38,$E$39)</f>
+        <v>-1.8034562997711343</v>
+      </c>
+      <c r="H24">
+        <v>0.17779335904242</v>
+      </c>
+      <c r="I24">
+        <v>0.66111840336646999</v>
+      </c>
+      <c r="L24">
+        <f>H24/B24</f>
+        <v>4.859685147159485E-2</v>
+      </c>
+      <c r="M24">
+        <f>STANDARDIZE(L24,$L$38,$L$39)</f>
+        <v>0.59230637368641692</v>
+      </c>
+      <c r="P24">
+        <f>B24+H24</f>
+        <v>3.8363299444082699</v>
+      </c>
+      <c r="Q24">
+        <f>STANDARDIZE(P24,$P$38,$P$39)</f>
+        <v>0.24375774740457481</v>
+      </c>
+      <c r="U24">
+        <f>(B24+H24)/B3</f>
+        <v>0.65108372290692651</v>
+      </c>
+      <c r="V24">
+        <f>STANDARDIZE(U24,$U$38,$U$39)</f>
+        <v>-1.9079786039820981</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>3.5092195291661801</v>
+      </c>
+      <c r="C25">
+        <v>-0.105042016666044</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.80952380952380831</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:F36" si="1">STANDARDIZE(E25,$E$38,$E$39)</f>
+        <v>-0.74439886174433756</v>
+      </c>
+      <c r="H25">
+        <v>4.6387568131740697E-3</v>
+      </c>
+      <c r="I25">
+        <v>-0.61498263991467295</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25:L36" si="2">H25/B25</f>
+        <v>1.3218770654329162E-3</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25:M36" si="3">STANDARDIZE(L25,$L$38,$L$39)</f>
+        <v>-0.55647665007588187</v>
+      </c>
+      <c r="P25">
+        <f t="shared" ref="P25:P36" si="4">B25+H25</f>
+        <v>3.5138582859793543</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" ref="Q25:Q36" si="5">STANDARDIZE(P25,$P$38,$P$39)</f>
+        <v>-0.22037091888914842</v>
+      </c>
+      <c r="U25">
+        <f>(B25+H25)/B4</f>
+        <v>0.81059390048153979</v>
+      </c>
+      <c r="V25">
+        <f>STANDARDIZE(U25,$U$38,$U$39)</f>
+        <v>-0.92201226183314622</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>2.93522685051397</v>
+      </c>
+      <c r="C26">
+        <v>-0.97052795401736802</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.1674876847290614</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1.2655454518030809</v>
+      </c>
+      <c r="H26">
+        <v>4.12830780663006E-3</v>
+      </c>
+      <c r="I26">
+        <v>-0.61874450648597101</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>1.406469760900142E-3</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
+        <v>-0.55442104552595373</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>2.9393551583206001</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="5"/>
+        <v>-1.0472447338498765</v>
+      </c>
+      <c r="U26">
+        <f>(B26+H26)/B5</f>
+        <v>1.1691297208538562</v>
+      </c>
+      <c r="V26">
+        <f>STANDARDIZE(U26,$U$38,$U$39)</f>
+        <v>1.2941739196191917</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>3.13563129854291</v>
+      </c>
+      <c r="C27">
+        <v>-0.66835122249708201</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0.94946550048590794</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>4.1364801743219395E-2</v>
+      </c>
+      <c r="H27">
+        <v>3.20944861672765E-3</v>
+      </c>
+      <c r="I27">
+        <v>-0.62551624200883305</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>1.0235414534288652E-3</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="3"/>
+        <v>-0.56372621267764011</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="4"/>
+        <v>3.1388407471596378</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>-0.76012809003762616</v>
+      </c>
+      <c r="U27">
+        <f>(B27+H27)/B6</f>
+        <v>0.950437317784256</v>
+      </c>
+      <c r="V27">
+        <f>STANDARDIZE(U27,$U$38,$U$39)</f>
+        <v>-5.7610348876383978E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>4.7503373819163297</v>
+      </c>
+      <c r="C28">
+        <v>1.7663582434787</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.98324022346368678</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0.23100771571575676</v>
+      </c>
+      <c r="H28">
+        <v>0.13495276653171401</v>
+      </c>
+      <c r="I28">
+        <v>0.34539520517323902</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>2.8409090909090929E-2</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="3"/>
+        <v>0.10174330277421514</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="4"/>
+        <v>4.8852901484480435</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>1.7535105823300412</v>
+      </c>
+      <c r="U28">
+        <f>(B28+H28)/B7</f>
+        <v>1.0111731843575416</v>
+      </c>
+      <c r="V28">
+        <f>STANDARDIZE(U28,$U$38,$U$39)</f>
+        <v>0.31781096350036231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>3.8397113773998202</v>
+      </c>
+      <c r="C29">
+        <v>0.39328497894494702</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0.96129032258064451</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0.10776042312930961</v>
+      </c>
+      <c r="H29">
+        <v>0.19327406262079599</v>
+      </c>
+      <c r="I29">
+        <v>0.77520686381026305</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>5.0335570469798571E-2</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="3"/>
+        <v>0.63455728748001761</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="4"/>
+        <v>4.0329854400206164</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="5"/>
+        <v>0.52680108008867643</v>
+      </c>
+      <c r="U29">
+        <f>(B29+H29)/B8</f>
+        <v>1.0096774193548381</v>
+      </c>
+      <c r="V29">
+        <f>STANDARDIZE(U29,$U$38,$U$39)</f>
+        <v>0.30856532180618218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>4.4935377216711796</v>
+      </c>
+      <c r="C30">
+        <v>1.37914686792482</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.0033557046979886</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0.34395485904962547</v>
+      </c>
+      <c r="H30">
+        <v>6.0114217012323397E-2</v>
+      </c>
+      <c r="I30">
+        <v>-0.20614399672971501</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>1.3377926421404665E-2</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
+        <v>-0.26351435855160499</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="4"/>
+        <v>4.5536519386835028</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="5"/>
+        <v>1.2761886349069176</v>
+      </c>
+      <c r="U30">
+        <f>(B30+H30)/B9</f>
+        <v>1.0167785234899349</v>
+      </c>
+      <c r="V30">
+        <f>STANDARDIZE(U30,$U$38,$U$39)</f>
+        <v>0.35245875717036229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>4.1599650844197296</v>
+      </c>
+      <c r="C31">
+        <v>0.87617455248654397</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.98923697866615456</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0.26467911345672956</v>
+      </c>
+      <c r="H31">
+        <v>4.5260937386342501E-2</v>
+      </c>
+      <c r="I31">
+        <v>-0.31560851793121603</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>1.088012434427822E-2</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="3"/>
+        <v>-0.32421100955914228</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>4.2052260218060722</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="5"/>
+        <v>0.77470439008874148</v>
+      </c>
+      <c r="U31">
+        <f>(B31+H31)/B10</f>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="V31">
+        <f>STANDARDIZE(U31,$U$38,$U$39)</f>
+        <v>0.24874713397758708</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>4.20446100438771</v>
+      </c>
+      <c r="C32">
+        <v>0.94326703368720899</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.96630790828264002</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.13593384661702893</v>
+      </c>
+      <c r="H32">
+        <v>3.5631025460912798E-2</v>
+      </c>
+      <c r="I32">
+        <v>-0.386578278460462</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>8.4745762711864406E-3</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="3"/>
+        <v>-0.38266588603289348</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="4"/>
+        <v>4.2400920298486229</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>0.82488651738208452</v>
+      </c>
+      <c r="U32">
+        <f>(B32+H32)/B11</f>
+        <v>0.9744969583528319</v>
+      </c>
+      <c r="V32">
+        <f>STANDARDIZE(U32,$U$38,$U$39)</f>
+        <v>9.1107407980986405E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>2.91238612134135</v>
+      </c>
+      <c r="C33">
+        <v>-1.00496799242374</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.0255972696245745</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.4688398266261834</v>
+      </c>
+      <c r="H33">
+        <v>4.8459003682884303E-3</v>
+      </c>
+      <c r="I33">
+        <v>-0.61345604978430801</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>1.6638935108153059E-3</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="3"/>
+        <v>-0.54816564216444019</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="4"/>
+        <v>2.9172320217096384</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>-1.0790862356410889</v>
+      </c>
+      <c r="U33">
+        <f>(B33+H33)/B12</f>
+        <v>1.0273037542662127</v>
+      </c>
+      <c r="V33">
+        <f>STANDARDIZE(U33,$U$38,$U$39)</f>
+        <v>0.41751744776022082</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>2.9486130735480001</v>
+      </c>
+      <c r="C34">
+        <v>-0.95034374571456404</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1.1122019635343623</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.95511965570302026</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>-0.64916898167290005</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="3"/>
+        <v>-0.58859829480113268</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="4"/>
+        <v>2.9486130735480001</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>-1.0339199540286423</v>
+      </c>
+      <c r="U34">
+        <f>(B34+H34)/B13</f>
+        <v>1.1122019635343623</v>
+      </c>
+      <c r="V34">
+        <f>STANDARDIZE(U34,$U$38,$U$39)</f>
+        <v>0.94229134068601006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>3.22622052971631</v>
+      </c>
+      <c r="C35">
+        <v>-0.53175765855102397</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.56564141035258697</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>-2.1137829681920279</v>
+      </c>
+      <c r="H35">
+        <v>0.47708698814770401</v>
+      </c>
+      <c r="I35">
+        <v>2.86682883457408</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>0.14787798408488073</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="3"/>
+        <v>3.0048403022329855</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>3.703307517864014</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>5.2300545491278987E-2</v>
+      </c>
+      <c r="U35">
+        <f>(B35+H35)/B14</f>
+        <v>0.64928732183045634</v>
+      </c>
+      <c r="V35">
+        <f>STANDARDIZE(U35,$U$38,$U$39)</f>
+        <v>-1.9190825412062369</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>2.75164136662067</v>
+      </c>
+      <c r="C36">
+        <v>-1.24734447192939</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>1.093023255813955</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0.84743243586353922</v>
+      </c>
+      <c r="H36">
+        <v>4.18182578513779E-3</v>
+      </c>
+      <c r="I36">
+        <v>-0.61835009393597895</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>1.5197568389057727E-3</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="3"/>
+        <v>-0.55166816678494401</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="4"/>
+        <v>2.7558231924058076</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>-1.3113995652459354</v>
+      </c>
+      <c r="U36">
+        <f>(B36+H36)/B15</f>
+        <v>1.0946843853820611</v>
+      </c>
+      <c r="V36">
+        <f>STANDARDIZE(U36,$U$38,$U$39)</f>
+        <v>0.83401146339696586</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <f>AVERAGE(B24:B36)</f>
+        <v>3.5788836865084619</v>
+      </c>
+      <c r="E38">
+        <f>AVERAGE(E24:E36)</f>
+        <v>0.94209857761680305</v>
+      </c>
+      <c r="H38">
+        <f>AVERAGE(H24:H36)</f>
+        <v>8.8085968891705446E-2</v>
+      </c>
+      <c r="L38">
+        <f>AVERAGE(L24:L36)</f>
+        <v>2.4222127892439795E-2</v>
+      </c>
+      <c r="P38">
+        <f>AVERAGE(P24:P36)</f>
+        <v>3.6669696554001678</v>
+      </c>
+      <c r="U38">
+        <f>AVERAGE(U24:U36)</f>
+        <v>0.95975755173806288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <f>_xlfn.STDEV.S(B24:B36)</f>
+        <v>0.6632027787867012</v>
+      </c>
+      <c r="E39">
+        <f>_xlfn.STDEV.S(E24:E36)</f>
+        <v>0.17809641430984252</v>
+      </c>
+      <c r="H39">
+        <f>_xlfn.STDEV.S(H24:H36)</f>
+        <v>0.13569035394252665</v>
+      </c>
+      <c r="L39">
+        <f>_xlfn.STDEV.S(L24:L36)</f>
+        <v>4.1152222332930179E-2</v>
+      </c>
+      <c r="P39">
+        <f>_xlfn.STDEV.S(P24:P36)</f>
+        <v>0.69478935874398196</v>
+      </c>
+      <c r="U39">
+        <f>_xlfn.STDEV.S(U24:U36)</f>
+        <v>0.16178055046681883</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E41" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>550</v>
+      </c>
+      <c r="B42">
+        <v>192</v>
+      </c>
+      <c r="C42">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>551</v>
+      </c>
+      <c r="B43" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>0.12771072269244299</v>
+      </c>
+      <c r="C44">
+        <v>1.7819317918631199</v>
+      </c>
+      <c r="E44">
+        <f>B44/B24</f>
+        <v>3.4907597535934455E-2</v>
+      </c>
+      <c r="F44">
+        <f>STANDARDIZE(E44,$E$58,$E$59)</f>
+        <v>1.751339001380636</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>6.9581352197610998E-3</v>
+      </c>
+      <c r="C45">
+        <v>-0.91290579332641897</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ref="E45:E56" si="6">B45/B25</f>
+        <v>1.9828155981493727E-3</v>
+      </c>
+      <c r="F45">
+        <f t="shared" ref="F45:F56" si="7">STANDARDIZE(E45,$E$58,$E$59)</f>
+        <v>-0.89366995376574232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>8.2566156132601199E-3</v>
+      </c>
+      <c r="C46">
+        <v>-0.88392758390440895</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="6"/>
+        <v>2.8129395218002839E-3</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="7"/>
+        <v>-0.82698203412858595</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>9.6283458501829396E-3</v>
+      </c>
+      <c r="C47">
+        <v>-0.85331465645855398</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="6"/>
+        <v>3.0706243602865923E-3</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="7"/>
+        <v>-0.80628094925307636</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>0.107962213225371</v>
+      </c>
+      <c r="C48">
+        <v>1.3412039641850899</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>2.27272727272727E-2</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="7"/>
+        <v>0.77283386636168427</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>5.1539750032212298E-2</v>
+      </c>
+      <c r="C49">
+        <v>8.2022876274273099E-2</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="6"/>
+        <v>1.3422818791946295E-2</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="7"/>
+        <v>2.5361520813907069E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>3.0057108506161698E-2</v>
+      </c>
+      <c r="C50">
+        <v>-0.397405606586618</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="6"/>
+        <v>6.6889632107023323E-3</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="7"/>
+        <v>-0.51560207155577686</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51">
+        <v>2.5055161767439601E-2</v>
+      </c>
+      <c r="C51">
+        <v>-0.50903413855223001</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="6"/>
+        <v>6.0229259762968725E-3</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="7"/>
+        <v>-0.56910810396602163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52">
+        <v>4.1739201254212099E-2</v>
+      </c>
+      <c r="C52">
+        <v>-0.136696140479</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="6"/>
+        <v>9.9273607748183931E-3</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="7"/>
+        <v>-0.2554457378374001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>3.8767202946307401E-2</v>
+      </c>
+      <c r="C53">
+        <v>-0.20302227817002999</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="6"/>
+        <v>1.3311148086522433E-2</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="7"/>
+        <v>1.6390466231624354E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>4.83379192384919E-2</v>
+      </c>
+      <c r="C54">
+        <v>1.0567563018254801E-2</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="6"/>
+        <v>1.6393442622950852E-2</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="7"/>
+        <v>0.26400627934945514</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55">
+        <v>0.126224808523384</v>
+      </c>
+      <c r="C55">
+        <v>1.7487706196269399</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="6"/>
+        <v>3.9124668435013422E-2</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="7"/>
+        <v>2.0901169563456259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>-1.0681906174904201</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="7"/>
+        <v>-1.0529592399763292</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <f>AVERAGE(B44:B56)</f>
+        <v>4.7864398836094398E-2</v>
+      </c>
+      <c r="E58">
+        <f>AVERAGE(E44:E56)</f>
+        <v>1.3107121357053384E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <f>_xlfn.STDEV.S(B44:B56)</f>
+        <v>4.4808855322607088E-2</v>
+      </c>
+      <c r="E59">
+        <f>_xlfn.STDEV.S(E44:E56)</f>
+        <v>1.2447890535010676E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E41:F41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K65" sqref="K65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>7</v>
+      </c>
+      <c r="F1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>5.8922221665748502</v>
+      </c>
+      <c r="C3">
+        <v>1.67865891138622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4.3349182419111703</v>
+      </c>
+      <c r="C4">
+        <v>0.318342770386637</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2.5141394542377098</v>
+      </c>
+      <c r="C5">
+        <v>-1.2721205520484899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3.3025226266127499</v>
+      </c>
+      <c r="C6">
+        <v>-0.58346219982232606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4.8313090418353601</v>
+      </c>
+      <c r="C7">
+        <v>0.75194369226602997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>3.9943306274964598</v>
+      </c>
+      <c r="C8">
+        <v>2.0837047852143201E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>4.4785091674180899</v>
+      </c>
+      <c r="C9">
+        <v>0.44377047308142398</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>4.2052260218060704</v>
+      </c>
+      <c r="C10">
+        <v>0.20505568648672901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>4.3510572234268903</v>
+      </c>
+      <c r="C11">
+        <v>0.33244028642537199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2.8396976158170202</v>
+      </c>
+      <c r="C12">
+        <v>-0.987743164297326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>2.65114895515728</v>
+      </c>
+      <c r="C13">
+        <v>-1.1524417709066199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>5.7036498224295098</v>
+      </c>
+      <c r="C14">
+        <v>1.5139396170824799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2.5174591226529501</v>
+      </c>
+      <c r="C15">
+        <v>-1.26922079789228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <f>AVERAGE(B3:B15)</f>
+        <v>3.9704761605673937</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <f>_xlfn.STDEV.S(B3:B15)</f>
+        <v>1.1448102964648721</v>
+      </c>
+    </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
-        <v>558</v>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>550</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>550</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
+        <v>551</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
       </c>
       <c r="E22" t="s">
         <v>553</v>
@@ -52735,275 +54038,1488 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>551</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1.4323633996093601</v>
+      </c>
+      <c r="C23">
+        <v>0.24394860989301401</v>
+      </c>
+      <c r="E23">
+        <f>B23/B3</f>
+        <v>0.24309392265193441</v>
+      </c>
+      <c r="F23">
+        <f>STANDARDIZE(E23,$E$37,$E$38)</f>
+        <v>-0.96878296439432199</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24">
-        <v>3.6585365853658498</v>
+        <v>1.3058100429085</v>
       </c>
       <c r="C24">
-        <v>0.120103385276993</v>
+        <v>-0.212636475773854</v>
       </c>
       <c r="E24">
-        <f>B24/B3</f>
-        <v>0.62090947726306756</v>
+        <f t="shared" ref="E24:E35" si="0">B24/B4</f>
+        <v>0.30123060460139084</v>
       </c>
       <c r="F24">
-        <f>STANDARDIZE(E24,$E$38,$E$39)</f>
-        <v>-1.8034562997711343</v>
+        <f t="shared" ref="F24:F35" si="1">STANDARDIZE(E24,$E$37,$E$38)</f>
+        <v>-0.52185913864462707</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25">
-        <v>3.5092195291661801</v>
+        <v>1.4614209635470401</v>
       </c>
       <c r="C25">
-        <v>-0.105042016666044</v>
+        <v>0.348783840388876</v>
       </c>
       <c r="E25">
-        <f>B25/B4</f>
-        <v>0.80952380952380831</v>
+        <f t="shared" si="0"/>
+        <v>0.58128078817733875</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25:F36" si="0">STANDARDIZE(E25,$E$38,$E$39)</f>
-        <v>-0.74439886174433756</v>
+        <f t="shared" si="1"/>
+        <v>1.6310174144837588</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26">
-        <v>2.93522685051397</v>
+        <v>1.4025290455099799</v>
       </c>
       <c r="C26">
-        <v>-0.97052795401736802</v>
+        <v>0.13631083972720401</v>
       </c>
       <c r="E26">
-        <f>B26/B5</f>
-        <v>1.1674876847290614</v>
+        <f t="shared" si="0"/>
+        <v>0.42468415937803622</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>1.2655454518030809</v>
+        <f t="shared" si="1"/>
+        <v>0.42718599350010039</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>3.13563129854291</v>
+        <v>1.88933873144399</v>
       </c>
       <c r="C27">
-        <v>-0.66835122249708201</v>
+        <v>1.89264546371542</v>
       </c>
       <c r="E27">
-        <f>B27/B6</f>
-        <v>0.94946550048590794</v>
+        <f t="shared" si="0"/>
+        <v>0.39106145251396535</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>4.1364801743219395E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.16871254300605171</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>4.7503373819163297</v>
+        <v>1.4946527509341601</v>
       </c>
       <c r="C28">
-        <v>1.7663582434787</v>
+        <v>0.46867902836777398</v>
       </c>
       <c r="E28">
-        <f>B28/B7</f>
-        <v>0.98324022346368678</v>
+        <f t="shared" si="0"/>
+        <v>0.37419354838709701</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>0.23100771571575676</v>
+        <f t="shared" si="1"/>
+        <v>3.9041086156946986E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29">
-        <v>3.8397113773998202</v>
+        <v>1.4277126540426801</v>
       </c>
       <c r="C29">
-        <v>0.39328497894494702</v>
+        <v>0.22716943375472901</v>
       </c>
       <c r="E29">
-        <f>B29/B8</f>
-        <v>0.96129032258064451</v>
+        <f t="shared" si="0"/>
+        <v>0.31879194630872493</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
-        <v>0.10776042312930961</v>
+        <f t="shared" si="1"/>
+        <v>-0.38685690325797528</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>4.4935377216711796</v>
+        <v>1.3085260290801499</v>
       </c>
       <c r="C30">
-        <v>1.37914686792482</v>
+        <v>-0.20283761455688201</v>
       </c>
       <c r="E30">
-        <f>B30/B9</f>
-        <v>1.0033557046979886</v>
+        <f t="shared" si="0"/>
+        <v>0.31116663463386474</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
-        <v>0.34395485904962547</v>
+        <f t="shared" si="1"/>
+        <v>-0.44547623535582637</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>4.1599650844197296</v>
+        <v>1.14019281474921</v>
       </c>
       <c r="C31">
-        <v>0.87617455248654397</v>
+        <v>-0.81015801355309602</v>
       </c>
       <c r="E31">
-        <f>B31/B10</f>
-        <v>0.98923697866615456</v>
+        <f t="shared" si="0"/>
+        <v>0.26204960224613977</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
-        <v>0.26467911345672956</v>
+        <f t="shared" si="1"/>
+        <v>-0.82306180247295624</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>1.13878658654778</v>
+      </c>
+      <c r="C32">
+        <v>-0.81523146905482302</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.40102389078498252</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.24529845875798773</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>1.75875659998513</v>
+      </c>
+      <c r="C33">
+        <v>1.4215251771185</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.66339410939691668</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>2.2622608641249449</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>1.17453254032776</v>
+      </c>
+      <c r="C34">
+        <v>-0.68626555464250305</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.20592648162040558</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>-1.2545064419326262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>0.80709237653159405</v>
+      </c>
+      <c r="C35">
+        <v>-2.01193326538435</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.32059800664451843</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>-0.37297287397145085</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <f>AVERAGE(B23:B35)</f>
+        <v>1.3647472719397948</v>
+      </c>
+      <c r="E37">
+        <f>AVERAGE(E23:E35)</f>
+        <v>0.36911501133425495</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <f>_xlfn.STDEV.S(B23:B35)</f>
+        <v>0.27717365431684315</v>
+      </c>
+      <c r="E38">
+        <f>_xlfn.STDEV.S(E23:E35)</f>
+        <v>0.13008185869691491</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="E43" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>550</v>
+      </c>
+      <c r="B44">
+        <v>26</v>
+      </c>
+      <c r="C44">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>551</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" t="s">
+        <v>553</v>
+      </c>
+      <c r="F45" t="s">
+        <v>554</v>
+      </c>
+      <c r="O45">
+        <v>32</v>
+      </c>
+      <c r="P45">
+        <v>32</v>
+      </c>
+      <c r="S45">
+        <v>53</v>
+      </c>
+      <c r="T45">
+        <v>53</v>
+      </c>
+      <c r="W45">
+        <v>85</v>
+      </c>
+      <c r="X45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>0.64857014073220798</v>
+      </c>
+      <c r="C46">
+        <v>1.39222740071604</v>
+      </c>
+      <c r="E46">
+        <f>B46/B23</f>
+        <v>0.4527972027972012</v>
+      </c>
+      <c r="F46">
+        <f>STANDARDIZE(E46,$E$60,$E$61)</f>
+        <v>2.0370195454999562</v>
+      </c>
+      <c r="O46" t="s">
+        <v>44</v>
+      </c>
+      <c r="P46" t="s">
+        <v>44</v>
+      </c>
+      <c r="S46" t="s">
+        <v>65</v>
+      </c>
+      <c r="T46" t="s">
+        <v>65</v>
+      </c>
+      <c r="W46" t="s">
+        <v>97</v>
+      </c>
+      <c r="X46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>0.38501681549344802</v>
+      </c>
+      <c r="C47">
+        <v>-0.214380627505111</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ref="E47:E58" si="2">B47/B24</f>
+        <v>0.29484902309058647</v>
+      </c>
+      <c r="F47">
+        <f t="shared" ref="F47:F58" si="3">STANDARDIZE(E47,$E$60,$E$61)</f>
+        <v>-6.1147383036993568E-2</v>
+      </c>
+      <c r="O47">
+        <v>0.202834677217409</v>
+      </c>
+      <c r="P47">
+        <v>-0.69888054425045498</v>
+      </c>
+      <c r="S47">
+        <v>0.12520659087494401</v>
+      </c>
+      <c r="T47">
+        <v>-0.56309510667684304</v>
+      </c>
+      <c r="W47">
+        <v>6.2603295437471798E-2</v>
+      </c>
+      <c r="X47">
+        <v>-0.57072185077953097</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>0.39218924162985602</v>
+      </c>
+      <c r="C48">
+        <v>-0.17065787271862801</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>0.26836158192090437</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>-0.41300375255656968</v>
+      </c>
+      <c r="O48">
+        <v>0.419807491592253</v>
+      </c>
+      <c r="P48">
+        <v>0.79885843728886397</v>
+      </c>
+      <c r="S48">
+        <v>0.14380146120839599</v>
+      </c>
+      <c r="T48">
+        <v>-0.38154081293761399</v>
+      </c>
+      <c r="W48">
+        <v>0.10437202829641699</v>
+      </c>
+      <c r="X48">
+        <v>-6.0592310210559899E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>0.34982989922331298</v>
+      </c>
+      <c r="C49">
+        <v>-0.42887832779680701</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>0.24942791762013725</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="3"/>
+        <v>-0.66451654837150342</v>
+      </c>
+      <c r="O49">
+        <v>0.44172893530941698</v>
+      </c>
+      <c r="P49">
+        <v>0.95017970249628203</v>
+      </c>
+      <c r="S49">
+        <v>0.16926062007183301</v>
+      </c>
+      <c r="T49">
+        <v>-0.13296582834465601</v>
+      </c>
+      <c r="W49">
+        <v>0.30962308549725498</v>
+      </c>
+      <c r="X49">
+        <v>2.4461781935715998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>0.75573549257759798</v>
+      </c>
+      <c r="C50">
+        <v>2.0455020822855898</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000102</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>1.3356670827231745</v>
+      </c>
+      <c r="O50">
+        <v>0.33699210475640301</v>
+      </c>
+      <c r="P50">
+        <v>0.22719311832855499</v>
+      </c>
+      <c r="S50">
+        <v>8.9864561268374096E-2</v>
+      </c>
+      <c r="T50">
+        <v>-0.90816324156930595</v>
+      </c>
+      <c r="W50">
+        <v>0.16047243083638199</v>
+      </c>
+      <c r="X50">
+        <v>0.62457265924382099</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>0.489627625306017</v>
+      </c>
+      <c r="C51">
+        <v>0.42332169224870803</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0.3275862068965511</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>0.37372990724072269</v>
+      </c>
+      <c r="O51">
+        <v>0.215924426450742</v>
+      </c>
+      <c r="P51">
+        <v>-0.60852347467090795</v>
+      </c>
+      <c r="S51">
+        <v>0.107962213225371</v>
+      </c>
+      <c r="T51">
+        <v>-0.73146362708046997</v>
+      </c>
+      <c r="W51">
+        <v>5.3981106612685598E-2</v>
+      </c>
+      <c r="X51">
+        <v>-0.67602629558375504</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52">
+        <v>0.55605650736399204</v>
+      </c>
+      <c r="C52">
+        <v>0.82826886991536297</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0.38947368421052692</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="3"/>
+        <v>1.1958366161116878</v>
+      </c>
+      <c r="O52">
+        <v>0.38654812524159299</v>
+      </c>
+      <c r="P52">
+        <v>0.56927276487083101</v>
+      </c>
+      <c r="S52">
+        <v>0.18038912511274299</v>
+      </c>
+      <c r="T52">
+        <v>-2.4310708042946001E-2</v>
+      </c>
+      <c r="W52">
+        <v>7.7309625048318495E-2</v>
+      </c>
+      <c r="X52">
+        <v>-0.39111062835695498</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53">
+        <v>0.37178627138781301</v>
+      </c>
+      <c r="C53">
+        <v>-0.29503336963458099</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0.2841260037059915</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="3"/>
+        <v>-0.20359083942002126</v>
+      </c>
+      <c r="O53">
+        <v>0.300571085061617</v>
+      </c>
+      <c r="P53">
+        <v>-2.4217092215389899E-2</v>
+      </c>
+      <c r="S53">
+        <v>0.48091373609858701</v>
+      </c>
+      <c r="T53">
+        <v>2.90991429704538</v>
+      </c>
+      <c r="W53">
+        <v>0.165314096783889</v>
+      </c>
+      <c r="X53">
+        <v>0.68370485350336696</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>8</v>
       </c>
-      <c r="B32">
-        <v>4.20446100438771</v>
-      </c>
-      <c r="C32">
-        <v>0.94326703368720899</v>
-      </c>
-      <c r="E32">
-        <f>B32/B11</f>
-        <v>0.96630790828264002</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>0.13593384661702893</v>
+      <c r="B54">
+        <v>0.28403017438841899</v>
+      </c>
+      <c r="C54">
+        <v>-0.82999019416660003</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0.24910714285714261</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="3"/>
+        <v>-0.66877768642624247</v>
+      </c>
+      <c r="O54">
+        <v>0.20933183541183401</v>
+      </c>
+      <c r="P54">
+        <v>-0.65403139056704895</v>
+      </c>
+      <c r="S54">
+        <v>0.24085284537732299</v>
+      </c>
+      <c r="T54">
+        <v>0.56603748114197106</v>
+      </c>
+      <c r="W54">
+        <v>3.7178627138781402E-2</v>
+      </c>
+      <c r="X54">
+        <v>-0.88123819807044401</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>9</v>
       </c>
-      <c r="B33">
-        <v>2.91238612134135</v>
-      </c>
-      <c r="C33">
-        <v>-1.00496799242374</v>
-      </c>
-      <c r="E33">
-        <f>B33/B12</f>
-        <v>1.0255972696245745</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>0.4688398266261834</v>
+      <c r="B55">
+        <v>0.26652452025586398</v>
+      </c>
+      <c r="C55">
+        <v>-0.93670379545828297</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0.23404255319148987</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="3"/>
+        <v>-0.86889410364082076</v>
+      </c>
+      <c r="O55">
+        <v>0.182227244500097</v>
+      </c>
+      <c r="P55">
+        <v>-0.84113133902903503</v>
+      </c>
+      <c r="S55">
+        <v>0.15677651202801601</v>
+      </c>
+      <c r="T55">
+        <v>-0.25485661748243998</v>
+      </c>
+      <c r="W55">
+        <v>1.8324527379897999E-2</v>
+      </c>
+      <c r="X55">
+        <v>-1.11150693234882</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>10</v>
       </c>
-      <c r="B34">
-        <v>2.9486130735480001</v>
-      </c>
-      <c r="C34">
-        <v>-0.95034374571456404</v>
-      </c>
-      <c r="E34">
-        <f>B34/B13</f>
-        <v>1.1122019635343623</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
-        <v>0.95511965570302026</v>
+      <c r="B56">
+        <v>0.472224287945267</v>
+      </c>
+      <c r="C56">
+        <v>0.31723180893460901</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0.26849894291754728</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="3"/>
+        <v>-0.41117906359236406</v>
+      </c>
+      <c r="O56">
+        <v>0.27137042062415201</v>
+      </c>
+      <c r="P56">
+        <v>-0.22578600093260501</v>
+      </c>
+      <c r="S56">
+        <v>0.15991471215351799</v>
+      </c>
+      <c r="T56">
+        <v>-0.22421624746744401</v>
+      </c>
+      <c r="W56">
+        <v>0.111455708470634</v>
+      </c>
+      <c r="X56">
+        <v>2.59220335454333E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>11</v>
       </c>
-      <c r="B35">
-        <v>3.22622052971631</v>
-      </c>
-      <c r="C35">
-        <v>-0.53175765855102397</v>
-      </c>
-      <c r="E35">
-        <f>B35/B14</f>
-        <v>0.56564141035258697</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>-2.1137829681920279</v>
+      <c r="B57">
+        <v>0.34444396902143698</v>
+      </c>
+      <c r="C57">
+        <v>-0.46171069177451302</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0.29326047358834173</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="3"/>
+        <v>-8.2249506759753774E-2</v>
+      </c>
+      <c r="O57">
+        <v>0.66185766341935004</v>
+      </c>
+      <c r="P57">
+        <v>2.4697036022846302</v>
+      </c>
+      <c r="S57">
+        <v>0.263999405071763</v>
+      </c>
+      <c r="T57">
+        <v>0.79203299616618394</v>
+      </c>
+      <c r="W57">
+        <v>0.20078827991373499</v>
+      </c>
+      <c r="X57">
+        <v>1.1169578517018199</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>12</v>
       </c>
-      <c r="B36">
-        <v>2.75164136662067</v>
-      </c>
-      <c r="C36">
-        <v>-1.24734447192939</v>
-      </c>
-      <c r="E36">
-        <f>B36/B15</f>
-        <v>1.093023255813955</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>0.84743243586353922</v>
+      <c r="B58">
+        <v>0.146363902479823</v>
+      </c>
+      <c r="C58">
+        <v>-1.66919697504579</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0.18134715025906767</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="3"/>
+        <v>-1.5688942677712781</v>
+      </c>
+      <c r="O58">
+        <v>0.17329168627786601</v>
+      </c>
+      <c r="P58">
+        <v>-0.90281249438395805</v>
+      </c>
+      <c r="S58">
+        <v>0.14975824740062499</v>
+      </c>
+      <c r="T58">
+        <v>-0.32338068110060803</v>
+      </c>
+      <c r="W58">
+        <v>3.2091053014419599E-2</v>
+      </c>
+      <c r="X58">
+        <v>-0.94337371602919595</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E38">
-        <f>AVERAGE(E24:E36)</f>
-        <v>0.94209857761680305</v>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <f>AVERAGE(B46:B58)</f>
+        <v>0.42018452675423507</v>
+      </c>
+      <c r="E60">
+        <f>AVERAGE(E46:E58)</f>
+        <v>0.29945214485042226</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E39">
-        <f>_xlfn.STDEV.S(E24:E36)</f>
-        <v>0.17809641430984252</v>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <f>_xlfn.STDEV.S(B46:B58)</f>
+        <v>0.16404332644258474</v>
+      </c>
+      <c r="E61">
+        <f>_xlfn.STDEV.S(E46:E58)</f>
+        <v>7.5279129395463246E-2</v>
+      </c>
+      <c r="O61">
+        <v>0.15054572826495999</v>
+      </c>
+      <c r="P61">
+        <v>-1.0598252892197599</v>
+      </c>
+      <c r="S61">
+        <v>0.10872747041358299</v>
+      </c>
+      <c r="T61">
+        <v>-0.72399190365120503</v>
+      </c>
+      <c r="W61">
+        <v>8.7818341487893595E-2</v>
+      </c>
+      <c r="X61">
+        <v>-0.262765660186775</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="E64" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>550</v>
+      </c>
+      <c r="B65">
+        <v>59</v>
+      </c>
+      <c r="C65">
+        <v>59</v>
+      </c>
+      <c r="O65">
+        <v>67</v>
+      </c>
+      <c r="P65">
+        <v>67</v>
+      </c>
+      <c r="S65">
+        <v>81</v>
+      </c>
+      <c r="T65">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>551</v>
+      </c>
+      <c r="B66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" t="s">
+        <v>553</v>
+      </c>
+      <c r="F66" t="s">
+        <v>554</v>
+      </c>
+      <c r="O66" t="s">
+        <v>79</v>
+      </c>
+      <c r="P66" t="s">
+        <v>79</v>
+      </c>
+      <c r="S66" t="s">
+        <v>93</v>
+      </c>
+      <c r="T66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>0.29548755446486702</v>
+      </c>
+      <c r="C67">
+        <v>1.2371899385204099</v>
+      </c>
+      <c r="E67">
+        <f>B67/B46</f>
+        <v>0.45559845559845569</v>
+      </c>
+      <c r="F67">
+        <f>STANDARDIZE(E67,$E$81,$E$82)</f>
+        <v>0.87936398934579163</v>
+      </c>
+      <c r="O67">
+        <v>8.7644613612460606E-2</v>
+      </c>
+      <c r="P67">
+        <v>-0.60028070313509097</v>
+      </c>
+      <c r="S67">
+        <v>6.0099163619973001E-2</v>
+      </c>
+      <c r="T67">
+        <v>-0.77610519292684399</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>0.10205264988983</v>
+      </c>
+      <c r="C68">
+        <v>-0.57217731769117597</v>
+      </c>
+      <c r="E68">
+        <f t="shared" ref="E68:E79" si="4">B68/B47</f>
+        <v>0.26506024096385644</v>
+      </c>
+      <c r="F68">
+        <f t="shared" ref="F68:F79" si="5">STANDARDIZE(E68,$E$81,$E$82)</f>
+        <v>-0.90594435724765543</v>
+      </c>
+      <c r="O68">
+        <v>0.21106343499942001</v>
+      </c>
+      <c r="P68">
+        <v>0.70731130438353595</v>
+      </c>
+      <c r="S68">
+        <v>8.5817001043720295E-2</v>
+      </c>
+      <c r="T68">
+        <v>-0.38738730453743098</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69">
+        <v>0.111464310779012</v>
+      </c>
+      <c r="C69">
+        <v>-0.48414175308164897</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="4"/>
+        <v>0.28421052631579025</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="5"/>
+        <v>-0.72650967353331908</v>
+      </c>
+      <c r="O69">
+        <v>0.23531354497791401</v>
+      </c>
+      <c r="P69">
+        <v>0.96423524542415195</v>
+      </c>
+      <c r="S69">
+        <v>0.17751723568509301</v>
+      </c>
+      <c r="T69">
+        <v>0.99863598300748702</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>9.9492907118557003E-2</v>
+      </c>
+      <c r="C70">
+        <v>-0.59612084931407405</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="4"/>
+        <v>0.28440366972477094</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="5"/>
+        <v>-0.72469995499048501</v>
+      </c>
+      <c r="O70">
+        <v>0.134796841902561</v>
+      </c>
+      <c r="P70">
+        <v>-0.10071446067749</v>
+      </c>
+      <c r="S70">
+        <v>6.4188972334552896E-2</v>
+      </c>
+      <c r="T70">
+        <v>-0.71428888305390903</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71">
+        <v>0.431848852901484</v>
+      </c>
+      <c r="C71">
+        <v>2.5126974222796301</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="4"/>
+        <v>0.57142857142857073</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="5"/>
+        <v>1.9646710652778412</v>
+      </c>
+      <c r="O71">
+        <v>0.107962213225371</v>
+      </c>
+      <c r="P71">
+        <v>-0.38502074061682601</v>
+      </c>
+      <c r="S71">
+        <v>0.13495276653171401</v>
+      </c>
+      <c r="T71">
+        <v>0.35528598832870201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>0.206159000128849</v>
+      </c>
+      <c r="C72">
+        <v>0.40162118935699997</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="4"/>
+        <v>0.42105263157894685</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="5"/>
+        <v>0.55567591406780403</v>
+      </c>
+      <c r="O72">
+        <v>0.25769875016106197</v>
+      </c>
+      <c r="P72">
+        <v>1.2014009795902201</v>
+      </c>
+      <c r="S72">
+        <v>0.14173431258858399</v>
+      </c>
+      <c r="T72">
+        <v>0.45778715200772602</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73">
+        <v>0.225428313796213</v>
+      </c>
+      <c r="C73">
+        <v>0.58186407404213003</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="4"/>
+        <v>0.40540540540540543</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="5"/>
+        <v>0.4090642564418997</v>
+      </c>
+      <c r="O73">
+        <v>0.165314096783889</v>
+      </c>
+      <c r="P73">
+        <v>0.22260833665437499</v>
+      </c>
+      <c r="S73">
+        <v>4.5085662759242598E-2</v>
+      </c>
+      <c r="T73">
+        <v>-1.0030300410685</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74">
+        <v>0.133358119084759</v>
+      </c>
+      <c r="C74">
+        <v>-0.27934965545468898</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="4"/>
+        <v>0.35869565217391303</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="5"/>
+        <v>-2.8597618743745348E-2</v>
+      </c>
+      <c r="O74">
+        <v>7.6781947351831095E-2</v>
+      </c>
+      <c r="P74">
+        <v>-0.71536797607385305</v>
+      </c>
+      <c r="S74">
+        <v>6.3850250955733198E-2</v>
+      </c>
+      <c r="T74">
+        <v>-0.71940856154622101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75">
+        <v>0.109947164279388</v>
+      </c>
+      <c r="C75">
+        <v>-0.498332962291413</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="4"/>
+        <v>0.38709677419354838</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="5"/>
+        <v>0.23751571863328394</v>
+      </c>
+      <c r="O75">
+        <v>5.5991611438577199E-2</v>
+      </c>
+      <c r="P75">
+        <v>-0.93563646323241401</v>
+      </c>
+      <c r="S75">
+        <v>5.8027670036343598E-2</v>
+      </c>
+      <c r="T75">
+        <v>-0.80741523655038305</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76">
+        <v>5.8150804419461098E-2</v>
+      </c>
+      <c r="C76">
+        <v>-0.98282999620262401</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="4"/>
+        <v>0.21818181818181767</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="5"/>
+        <v>-1.3451866353828299</v>
+      </c>
+      <c r="O76">
+        <v>8.2380306260903299E-2</v>
+      </c>
+      <c r="P76">
+        <v>-0.656054742626487</v>
+      </c>
+      <c r="S76">
+        <v>0.188990114363249</v>
+      </c>
+      <c r="T76">
+        <v>1.1720453214382001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77">
+        <v>0.137577154755708</v>
+      </c>
+      <c r="C77">
+        <v>-0.23988529398087099</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="4"/>
+        <v>0.291338582677166</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="5"/>
+        <v>-0.65972108447596256</v>
+      </c>
+      <c r="O77">
+        <v>0.35323864058897902</v>
+      </c>
+      <c r="P77">
+        <v>2.2136225817643398</v>
+      </c>
+      <c r="S77">
+        <v>0.263999405071763</v>
+      </c>
+      <c r="T77">
+        <v>2.3057896800084898</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78">
+        <v>0.17329168627786601</v>
+      </c>
+      <c r="C78">
+        <v>9.4184216633547493E-2</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="4"/>
+        <v>0.50310559006211242</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="5"/>
+        <v>1.3244971813585098</v>
+      </c>
+      <c r="O78">
+        <v>4.9206281288776701E-2</v>
+      </c>
+      <c r="P78">
+        <v>-1.0075253645567599</v>
+      </c>
+      <c r="S78">
+        <v>6.4182106028839198E-2</v>
+      </c>
+      <c r="T78">
+        <v>-0.71439266533599199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79">
+        <v>3.7636432066240101E-2</v>
+      </c>
+      <c r="C79">
+        <v>-1.1747190128162299</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="4"/>
+        <v>0.25714285714285645</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="5"/>
+        <v>-0.98012880075113973</v>
+      </c>
+      <c r="O79">
+        <v>5.8545560991929098E-2</v>
+      </c>
+      <c r="P79">
+        <v>-0.90857799689770402</v>
+      </c>
+      <c r="S79">
+        <v>0.100363818843307</v>
+      </c>
+      <c r="T79">
+        <v>-0.16751623977132701</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <f>AVERAGE(B67:B79)</f>
+        <v>0.16322268845863341</v>
+      </c>
+      <c r="E81">
+        <f>AVERAGE(E67:E79)</f>
+        <v>0.36174775195747777</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <f>_xlfn.STDEV.S(B67:B79)</f>
+        <v>0.10690748597940644</v>
+      </c>
+      <c r="E82">
+        <f>_xlfn.STDEV.S(E67:E79)</f>
+        <v>0.10672566170329392</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>550</v>
+      </c>
+      <c r="F84">
+        <v>75</v>
+      </c>
+      <c r="J84">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>551</v>
+      </c>
+      <c r="F85" t="s">
+        <v>87</v>
+      </c>
+      <c r="J85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0.102669404517454</v>
+      </c>
+      <c r="J86">
+        <v>-0.19215574377137901</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>0.10205264988983</v>
+      </c>
+      <c r="J87">
+        <v>-0.19840263952690901</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F88">
+        <v>9.9079387359121501E-2</v>
+      </c>
+      <c r="J88">
+        <v>-0.22851779432469899</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="F89">
+        <v>3.53039347840041E-2</v>
+      </c>
+      <c r="J89">
+        <v>-0.87447744530157301</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="F90">
+        <v>0.16194331983805699</v>
+      </c>
+      <c r="J90">
+        <v>0.40820938272351398</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91">
+        <v>0.41231800025769899</v>
+      </c>
+      <c r="J91">
+        <v>2.9441685119327299</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="F92">
+        <v>3.0057108506161698E-2</v>
+      </c>
+      <c r="J92">
+        <v>-0.92762074627900504</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93">
+        <v>0.105070033218295</v>
+      </c>
+      <c r="J93">
+        <v>-0.16784060032501899</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94">
+        <v>7.3298109519591995E-2</v>
+      </c>
+      <c r="J94">
+        <v>-0.48964750117146699</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95">
+        <v>0.13083930994378801</v>
+      </c>
+      <c r="J95">
+        <v>9.31675513602922E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96">
+        <v>0.18963337547408299</v>
+      </c>
+      <c r="J96">
+        <v>0.68867244416726403</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>11</v>
+      </c>
+      <c r="F97">
+        <v>4.7066877754482102E-2</v>
+      </c>
+      <c r="J97">
+        <v>-0.75533463676217305</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98">
+        <v>9.2000167273031397E-2</v>
+      </c>
+      <c r="J98">
+        <v>-0.30022078272157698</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>